<commit_message>
Push the 2 test cases for screenings - view clients
Overall test cases for Screenings ignore first especially view clients
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 6/Iteration 6 Test Cases v2.xlsx
+++ b/Test Cases/Iteration 6/Iteration 6 Test Cases v2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smu/Desktop/Ulink/Test Cases/Iteration 6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shu Yan\Desktop\Ulink\Test Cases\Iteration 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="1420" windowWidth="25520" windowHeight="15540" tabRatio="674" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="4880" yWindow="1420" windowWidth="25520" windowHeight="15540" tabRatio="674" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Client -  CRUD" sheetId="17" state="hidden" r:id="rId1"/>
     <sheet name="Login &amp; Account Management" sheetId="21" r:id="rId2"/>
-    <sheet name="Screenings" sheetId="23" r:id="rId3"/>
-    <sheet name="Bootstrap" sheetId="22" r:id="rId4"/>
+    <sheet name="Bootstrap" sheetId="22" r:id="rId3"/>
+    <sheet name="Screenings" sheetId="23" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="133">
   <si>
     <t>No</t>
   </si>
@@ -548,32 +548,6 @@
     <t>The screening table should show screenings belonging to male, age group between 20 - 30 years old</t>
   </si>
   <si>
-    <t xml:space="preserve">Access the URL: viewscreenings.jsp 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Access the URL: viewscreenings.jsp
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Access the URL: viewscreenings.jsp 
-Demographic: Infant 
-Age Group: 0 - 10 in drop down list  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Access the URL: viewscreenings.jsp
-Demographic: Infant 
-Age Group: 20 - 30 in drop down list  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Access the URL: viewscreenings.jsp
-Demographic: Male
-Age Group: 20 - 30 in drop down list  
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">The screening table should show no result  / user not able to select any age in the drop down list </t>
   </si>
   <si>
@@ -613,11 +587,60 @@
   <si>
     <t>Page should direct to user home page</t>
   </si>
+  <si>
+    <t xml:space="preserve">Access the URL: viewscreenings.html
+Demographic: Male
+Age Group: 20 - 30 in drop down list  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access the URL: viewscreenings.html
+Demographic: Infant 
+Age Group: 20 - 30 in drop down list  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access the URL: viewscreenings.html
+Demographic: Infant 
+Age Group: 0 - 10 in drop down list  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access the URL: viewscreenings.html
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access the URL: viewscreenings.html 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59 Names should shown. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access the URL: viewscreenings.html
+Demographic: Male
+Age Group: 20 - 30 in drop down list  
+Illness: Cancers, Click 'View Client List' 
+</t>
+  </si>
+  <si>
+    <t>View Clients Base on Filter</t>
+  </si>
+  <si>
+    <t>6 Names should shown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access the URL: viewscreenings.html
+Demographic: Infant
+Illness: Fever, Click 'View Client List' 
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -720,6 +743,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3552995</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3715307</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B78076E-362F-4340-80F5-2861C6BC5F76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4540250" y="12617450"/>
+          <a:ext cx="3432345" cy="3499407"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>106458</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>223370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2576607</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2300541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53A9BCE6-A192-4E68-B4E1-B150F7F72B7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4521576" y="16427076"/>
+          <a:ext cx="2470149" cy="2077171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,7 +1107,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
@@ -1000,7 +1116,7 @@
     <col min="5" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="155" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1040,7 +1156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="155" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1060,7 +1176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1068,7 +1184,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1076,7 +1192,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1084,7 +1200,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1092,7 +1208,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1100,7 +1216,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1108,7 +1224,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1116,7 +1232,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1124,7 +1240,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1132,7 +1248,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1140,7 +1256,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1148,7 +1264,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1156,7 +1272,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1164,7 +1280,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1172,7 +1288,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1180,7 +1296,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1188,7 +1304,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1196,7 +1312,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1204,7 +1320,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1212,7 +1328,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1220,7 +1336,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1228,7 +1344,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1236,7 +1352,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1253,11 +1369,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
-      <selection sqref="A1:G25"/>
+    <sheetView topLeftCell="A4" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="8" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="8" customWidth="1"/>
@@ -1267,7 +1383,7 @@
     <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1309,7 +1425,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1328,7 +1444,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1350,7 +1466,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1372,7 +1488,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="93" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1394,7 +1510,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1416,7 +1532,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1438,7 +1554,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1460,7 +1576,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1482,7 +1598,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1504,7 +1620,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1526,7 +1642,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1548,7 +1664,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="93" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1570,7 +1686,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="124" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1592,7 +1708,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1614,7 +1730,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1636,7 +1752,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1658,7 +1774,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1680,7 +1796,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1702,21 +1818,21 @@
       <c r="I20" s="2"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1724,21 +1840,21 @@
       <c r="I21" s="2"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1746,21 +1862,21 @@
       <c r="I22" s="2"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1768,21 +1884,21 @@
       <c r="I23" s="2"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1790,21 +1906,21 @@
       <c r="I24" s="2"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="93" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1812,7 +1928,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="2"/>
@@ -1824,7 +1940,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="2"/>
@@ -1836,7 +1952,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="2"/>
@@ -1848,7 +1964,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="2"/>
@@ -1860,7 +1976,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="2"/>
@@ -1872,7 +1988,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="2"/>
@@ -1884,7 +2000,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="2"/>
@@ -1896,7 +2012,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="2"/>
@@ -1908,7 +2024,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="2"/>
@@ -1920,7 +2036,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="2"/>
@@ -1932,7 +2048,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="2"/>
@@ -1944,7 +2060,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="2"/>
@@ -1956,7 +2072,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="2"/>
@@ -1968,7 +2084,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="2"/>
@@ -1980,7 +2096,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="2"/>
@@ -1992,7 +2108,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="2"/>
@@ -2004,7 +2120,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="2"/>
@@ -2016,7 +2132,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="2"/>
@@ -2028,7 +2144,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="2"/>
@@ -2040,7 +2156,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="2"/>
@@ -2052,7 +2168,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="2"/>
@@ -2064,7 +2180,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="2"/>
@@ -2076,7 +2192,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="2"/>
@@ -2088,7 +2204,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="2"/>
@@ -2100,7 +2216,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="2"/>
@@ -2112,7 +2228,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="2"/>
@@ -2124,7 +2240,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="2"/>
@@ -2136,7 +2252,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="2"/>
@@ -2148,7 +2264,7 @@
       <c r="I53" s="2"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="5"/>
@@ -2159,7 +2275,7 @@
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="5"/>
@@ -2170,7 +2286,7 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="5"/>
@@ -2181,7 +2297,7 @@
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="5"/>
@@ -2192,7 +2308,7 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="5"/>
@@ -2203,7 +2319,7 @@
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="5"/>
@@ -2214,7 +2330,7 @@
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="5"/>
@@ -2225,7 +2341,7 @@
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="5"/>
@@ -2236,7 +2352,7 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="5"/>
@@ -2247,7 +2363,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="5"/>
@@ -2258,7 +2374,7 @@
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="5"/>
@@ -2269,7 +2385,7 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="5"/>
@@ -2280,7 +2396,7 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="5"/>
@@ -2291,7 +2407,7 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="5"/>
@@ -2302,7 +2418,7 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="5"/>
@@ -2313,7 +2429,7 @@
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="5"/>
@@ -2324,7 +2440,7 @@
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="5"/>
@@ -2335,7 +2451,7 @@
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="5"/>
@@ -2346,7 +2462,7 @@
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="5"/>
@@ -2357,7 +2473,7 @@
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="5"/>
@@ -2368,7 +2484,7 @@
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="5"/>
@@ -2379,7 +2495,7 @@
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="5"/>
@@ -2390,7 +2506,7 @@
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="5"/>
@@ -2401,7 +2517,7 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="5"/>
@@ -2412,7 +2528,7 @@
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="5"/>
@@ -2423,7 +2539,7 @@
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="5"/>
@@ -2434,7 +2550,7 @@
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="5"/>
@@ -2445,7 +2561,7 @@
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="5"/>
@@ -2456,7 +2572,7 @@
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="5"/>
@@ -2467,7 +2583,7 @@
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="5"/>
@@ -2478,7 +2594,7 @@
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="5"/>
@@ -2489,7 +2605,7 @@
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="5"/>
@@ -2500,7 +2616,7 @@
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="5"/>
@@ -2511,7 +2627,7 @@
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="5"/>
@@ -2522,7 +2638,7 @@
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="5"/>
@@ -2533,7 +2649,7 @@
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="5"/>
@@ -2544,7 +2660,7 @@
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="5"/>
@@ -2555,7 +2671,7 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="5"/>
@@ -2566,7 +2682,7 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="5"/>
@@ -2577,7 +2693,7 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="5"/>
@@ -2588,7 +2704,7 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="5"/>
@@ -2599,7 +2715,7 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="5"/>
@@ -2610,7 +2726,7 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="5"/>
@@ -2621,7 +2737,7 @@
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="5"/>
@@ -2632,7 +2748,7 @@
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="5"/>
@@ -2643,7 +2759,7 @@
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="5"/>
@@ -2654,7 +2770,7 @@
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="5"/>
@@ -2665,7 +2781,7 @@
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="5"/>
@@ -2676,7 +2792,7 @@
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="5"/>
@@ -2687,7 +2803,7 @@
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="5"/>
@@ -2698,7 +2814,7 @@
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="5"/>
@@ -2709,7 +2825,7 @@
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="9"/>
       <c r="B105" s="9"/>
       <c r="C105" s="5"/>
@@ -2720,7 +2836,7 @@
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
       <c r="B106" s="9"/>
       <c r="C106" s="5"/>
@@ -2731,7 +2847,7 @@
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="9"/>
       <c r="C107" s="5"/>
@@ -2742,7 +2858,7 @@
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
       <c r="B108" s="9"/>
       <c r="C108" s="5"/>
@@ -2753,7 +2869,7 @@
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="9"/>
       <c r="B109" s="9"/>
       <c r="C109" s="5"/>
@@ -2764,7 +2880,7 @@
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="9"/>
       <c r="B110" s="9"/>
       <c r="C110" s="5"/>
@@ -2775,7 +2891,7 @@
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="9"/>
       <c r="B111" s="9"/>
       <c r="C111" s="5"/>
@@ -2786,7 +2902,7 @@
       <c r="H111" s="5"/>
       <c r="I111" s="5"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
       <c r="B112" s="9"/>
       <c r="C112" s="5"/>
@@ -2797,7 +2913,7 @@
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="9"/>
       <c r="B113" s="9"/>
       <c r="C113" s="5"/>
@@ -2808,7 +2924,7 @@
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="9"/>
       <c r="B114" s="9"/>
       <c r="C114" s="5"/>
@@ -2819,7 +2935,7 @@
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="9"/>
       <c r="B115" s="9"/>
       <c r="C115" s="5"/>
@@ -2830,7 +2946,7 @@
       <c r="H115" s="5"/>
       <c r="I115" s="5"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
       <c r="B116" s="9"/>
       <c r="C116" s="5"/>
@@ -2841,7 +2957,7 @@
       <c r="H116" s="5"/>
       <c r="I116" s="5"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="9"/>
       <c r="B117" s="9"/>
       <c r="C117" s="5"/>
@@ -2852,7 +2968,7 @@
       <c r="H117" s="5"/>
       <c r="I117" s="5"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="9"/>
       <c r="B118" s="9"/>
       <c r="C118" s="5"/>
@@ -2863,7 +2979,7 @@
       <c r="H118" s="5"/>
       <c r="I118" s="5"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="9"/>
       <c r="B119" s="9"/>
       <c r="C119" s="5"/>
@@ -2874,7 +2990,7 @@
       <c r="H119" s="5"/>
       <c r="I119" s="5"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="9"/>
       <c r="B120" s="9"/>
       <c r="C120" s="5"/>
@@ -2885,7 +3001,7 @@
       <c r="H120" s="5"/>
       <c r="I120" s="5"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="9"/>
       <c r="B121" s="9"/>
       <c r="C121" s="5"/>
@@ -2896,7 +3012,7 @@
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="9"/>
       <c r="B122" s="9"/>
       <c r="C122" s="5"/>
@@ -2907,7 +3023,7 @@
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="9"/>
       <c r="B123" s="9"/>
       <c r="C123" s="5"/>
@@ -2918,7 +3034,7 @@
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="9"/>
       <c r="B124" s="9"/>
       <c r="C124" s="5"/>
@@ -2929,7 +3045,7 @@
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="9"/>
       <c r="B125" s="9"/>
       <c r="C125" s="5"/>
@@ -2940,7 +3056,7 @@
       <c r="H125" s="5"/>
       <c r="I125" s="5"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="9"/>
       <c r="B126" s="9"/>
       <c r="C126" s="5"/>
@@ -2951,7 +3067,7 @@
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="9"/>
       <c r="B127" s="9"/>
       <c r="C127" s="5"/>
@@ -2962,7 +3078,7 @@
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="9"/>
       <c r="B128" s="9"/>
       <c r="C128" s="5"/>
@@ -2973,7 +3089,7 @@
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="9"/>
       <c r="B129" s="9"/>
       <c r="C129" s="5"/>
@@ -2984,7 +3100,7 @@
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="9"/>
       <c r="B130" s="9"/>
       <c r="C130" s="5"/>
@@ -2995,7 +3111,7 @@
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="9"/>
       <c r="B131" s="9"/>
       <c r="C131" s="5"/>
@@ -3006,7 +3122,7 @@
       <c r="H131" s="5"/>
       <c r="I131" s="5"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
@@ -3022,309 +3138,215 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.83203125" customWidth="1"/>
+    <col min="5" max="5" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    </row>
+    <row r="2" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="B2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="B3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="B4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="B5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="B6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="B7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="B8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" ht="112" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="B9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="B10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="B11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="B12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3333,217 +3355,345 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="36.83203125" customWidth="1"/>
-    <col min="5" max="5" width="48.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" customWidth="1"/>
+    <col min="4" max="4" width="57" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="B2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="B5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="B6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="B7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="B8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="B9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="B10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="B11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="300" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="196.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>